<commit_message>
oppdaterte kalender med paaske
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V25.xlsx
+++ b/diverse/tidsplan-V25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E369630-2FEA-4A24-B5E7-9A3EFAC6229A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66842A8-864F-4D50-9EDD-4A74776F470C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="25996" windowHeight="10276" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Uke</t>
   </si>
@@ -158,19 +158,28 @@
     <t xml:space="preserve"> 09.04: **Oppgaveseminar  6**, Aud A. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>14.04: **Speedrun anlyser**</t>
-  </si>
-  <si>
-    <t>16.04: **Speedrun anlyser**</t>
-  </si>
-  <si>
     <t>26.03 (Ingen aktivitet)</t>
   </si>
   <si>
     <t>31.03: (Ingen aktivitet)</t>
   </si>
   <si>
-    <t>Dataøving 5/Forberedelse til eksamen</t>
+    <t>14.04: (PÅSKE)</t>
+  </si>
+  <si>
+    <t>16.04: (PÅSKE)</t>
+  </si>
+  <si>
+    <t>Forberedelse til eksamen</t>
+  </si>
+  <si>
+    <t>Dataøving 5</t>
+  </si>
+  <si>
+    <t>21.04: **Speedrun anlyser**</t>
+  </si>
+  <si>
+    <t>23.04: **Speedrun anlyser**</t>
   </si>
 </sst>
 </file>
@@ -536,20 +545,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D0459C-A0F7-4603-AE4B-86A7155DF567}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="41.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2</v>
       </c>
@@ -577,7 +586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -591,7 +600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>4</v>
       </c>
@@ -605,7 +614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -619,7 +628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -633,7 +642,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -647,7 +656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -661,7 +670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -675,7 +684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -689,7 +698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>11</v>
       </c>
@@ -703,7 +712,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>12</v>
       </c>
@@ -717,7 +726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>13</v>
       </c>
@@ -728,10 +737,10 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>14</v>
       </c>
@@ -739,13 +748,13 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>15</v>
       </c>
@@ -759,18 +768,32 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>